<commit_message>
Adding labor force participation to population pyramid workforce figure
</commit_message>
<xml_diff>
--- a/analysis_data/age_generation_key.xlsx
+++ b/analysis_data/age_generation_key.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vandalsuidaho-my.sharepoint.com/personal/elizabethbageant_uidaho_edu/Documents/MAIN/Projects/Growth in Idaho 2024/Pop_Change_Analysis4/analysis_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{4EAD83AD-E1F0-E84A-9BBD-BDDFA265C6F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AB076EA9-001F-AC43-A14F-181BFB497A47}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{4EAD83AD-E1F0-E84A-9BBD-BDDFA265C6F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{16D23EC3-D15E-434A-ADF5-1E6EED35C5A8}"/>
   <bookViews>
     <workbookView xWindow="3560" yWindow="25020" windowWidth="27240" windowHeight="16440" xr2:uid="{15325187-6081-944C-9B27-CE4853469BA9}"/>
   </bookViews>
@@ -510,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A27369C2-F091-934C-8927-B6E955627C9F}">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -521,7 +521,7 @@
     <col min="1" max="1" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -532,7 +532,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -543,7 +543,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -554,7 +554,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -565,7 +565,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -576,7 +576,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -587,7 +587,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -597,12 +597,8 @@
       <c r="C7" t="s">
         <v>11</v>
       </c>
-      <c r="J7">
-        <f>280+380</f>
-        <v>660</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -613,7 +609,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -624,7 +620,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
@@ -635,7 +631,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
@@ -646,7 +642,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
@@ -657,7 +653,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
@@ -668,7 +664,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
@@ -679,7 +675,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>22</v>
       </c>
@@ -690,7 +686,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>24</v>
       </c>

</xml_diff>